<commit_message>
Update rapport_northwind.xlsx with new data and analysis
</commit_message>
<xml_diff>
--- a/reports/rapport_northwind.xlsx
+++ b/reports/rapport_northwind.xlsx
@@ -472,7 +472,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8934.699999999999</v>
+        <v>6979.6</v>
       </c>
       <c r="B2" t="n">
         <v>48</v>
@@ -484,10 +484,10 @@
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>186.1395833333333</v>
+        <v>145.4083333333333</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6476190476190476</v>
+        <v>0.9204545454545454</v>
       </c>
     </row>
   </sheetData>
@@ -544,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>723</v>
+        <v>681.2</v>
       </c>
       <c r="D2" t="n">
         <v>4</v>
@@ -561,13 +561,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>615</v>
+        <v>348.7</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -578,13 +578,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>1285.6</v>
+        <v>877.9</v>
       </c>
       <c r="D4" t="n">
         <v>8</v>
       </c>
       <c r="E4" t="n">
-        <v>92</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
@@ -595,13 +595,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>3052.5</v>
+        <v>3025.7</v>
       </c>
       <c r="D5" t="n">
         <v>17</v>
       </c>
       <c r="E5" t="n">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6">
@@ -612,13 +612,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>1781.7</v>
+        <v>994.9</v>
       </c>
       <c r="D6" t="n">
         <v>8</v>
       </c>
       <c r="E6" t="n">
-        <v>118</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7">
@@ -629,13 +629,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1476.9</v>
+        <v>1051.2</v>
       </c>
       <c r="D7" t="n">
         <v>8</v>
       </c>
       <c r="E7" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -682,33 +682,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Condiments</t>
+          <t>Beverages</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4631.8</v>
+        <v>4362.3</v>
       </c>
       <c r="C2" t="n">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D2" t="n">
-        <v>351</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Beverages</t>
+          <t>Condiments</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4302.9</v>
+        <v>2617.3</v>
       </c>
       <c r="C3" t="n">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D3" t="n">
-        <v>263</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -759,10 +759,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4302.9</v>
+        <v>4362.3</v>
       </c>
       <c r="C2" t="n">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D2" t="n">
         <v>48</v>
@@ -771,33 +771,33 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Northwind Traders Cajun Seasoning</t>
+          <t>Northwind Traders Syrup</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2467.3</v>
+        <v>1332.5</v>
       </c>
       <c r="C3" t="n">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="D3" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Northwind Traders Syrup</t>
+          <t>Northwind Traders Cajun Seasoning</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2164.5</v>
+        <v>1284.8</v>
       </c>
       <c r="C4" t="n">
-        <v>232</v>
+        <v>63</v>
       </c>
       <c r="D4" t="n">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8934.700000000001</v>
+        <v>6979.6</v>
       </c>
       <c r="C2" t="n">
         <v>48</v>
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2192.3</v>
+        <v>1598.1</v>
       </c>
       <c r="C2" t="n">
         <v>12</v>
@@ -917,33 +917,33 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Anne Hellung-Larsen</t>
+          <t>Mariya Sergienko</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1674.6</v>
+        <v>1526.1</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mariya Sergienko</t>
+          <t>Anne Hellung-Larsen</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1578.9</v>
+        <v>1332.2</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -953,7 +953,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1359.9</v>
+        <v>945.9</v>
       </c>
       <c r="C5" t="n">
         <v>6</v>
@@ -969,7 +969,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>932.7</v>
+        <v>701.2</v>
       </c>
       <c r="C6" t="n">
         <v>4</v>
@@ -981,43 +981,43 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Laura Giussani</t>
+          <t>Andrew Cencini</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>449.7</v>
+        <v>419.8</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Andrew Cencini</t>
+          <t>Robert Zare</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>414.5</v>
+        <v>254.7</v>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Robert Zare</t>
+          <t>Laura Giussani</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>332.1</v>
+        <v>201.6</v>
       </c>
       <c r="C9" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
feat: Enhance data extraction and transformation processes
- Updated `extract.py` to normalize SupplierID by converting to numeric and dropping invalid entries.
- Enhanced `transform.py` to parse additional date fields (InvoiceDate, DueDate) and implement targeted imputations for critical columns (Notes, TaxStatus, InvoiceDate, DueDate, PaidDate, ShippedDate).
- Added a new CSV file `supplier_analysis.csv` containing supplier details for improved data analysis.
</commit_message>
<xml_diff>
--- a/reports/rapport_northwind.xlsx
+++ b/reports/rapport_northwind.xlsx
@@ -472,7 +472,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6979.6</v>
+        <v>7831.599999999999</v>
       </c>
       <c r="B2" t="n">
         <v>48</v>
@@ -484,10 +484,10 @@
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>145.4083333333333</v>
+        <v>163.1583333333333</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9204545454545454</v>
+        <v>0.8712871287128713</v>
       </c>
     </row>
   </sheetData>
@@ -544,13 +544,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>681.2</v>
+        <v>717.1</v>
       </c>
       <c r="D2" t="n">
         <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
@@ -561,13 +561,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>348.7</v>
+        <v>861.0999999999999</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -578,13 +578,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>877.9</v>
+        <v>1069.3</v>
       </c>
       <c r="D4" t="n">
         <v>8</v>
       </c>
       <c r="E4" t="n">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
@@ -595,13 +595,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>3025.7</v>
+        <v>2690.3</v>
       </c>
       <c r="D5" t="n">
         <v>17</v>
       </c>
       <c r="E5" t="n">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6">
@@ -612,13 +612,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>994.9</v>
+        <v>1418.3</v>
       </c>
       <c r="D6" t="n">
         <v>8</v>
       </c>
       <c r="E6" t="n">
-        <v>68</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7">
@@ -629,13 +629,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1051.2</v>
+        <v>1075.5</v>
       </c>
       <c r="D7" t="n">
         <v>8</v>
       </c>
       <c r="E7" t="n">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -686,13 +686,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4362.3</v>
+        <v>4541.4</v>
       </c>
       <c r="C2" t="n">
         <v>48</v>
       </c>
       <c r="D2" t="n">
-        <v>262</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3">
@@ -702,13 +702,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2617.3</v>
+        <v>3290.2</v>
       </c>
       <c r="C3" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D3" t="n">
-        <v>208</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -759,10 +759,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4362.3</v>
+        <v>4541.4</v>
       </c>
       <c r="C2" t="n">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="D2" t="n">
         <v>48</v>
@@ -775,13 +775,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1332.5</v>
+        <v>1847</v>
       </c>
       <c r="C3" t="n">
-        <v>145</v>
+        <v>203</v>
       </c>
       <c r="D3" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
@@ -791,13 +791,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1284.8</v>
+        <v>1443.2</v>
       </c>
       <c r="C4" t="n">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D4" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6979.6</v>
+        <v>7831.6</v>
       </c>
       <c r="C2" t="n">
         <v>48</v>
@@ -901,49 +901,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nancy Freehafer</t>
+          <t>Anne Hellung-Larsen</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1598.1</v>
+        <v>1941.1</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mariya Sergienko</t>
+          <t>Nancy Freehafer</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1526.1</v>
+        <v>1826.5</v>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Anne Hellung-Larsen</t>
+          <t>Mariya Sergienko</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1332.2</v>
+        <v>1415.3</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -953,7 +953,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>945.9</v>
+        <v>950.3</v>
       </c>
       <c r="C5" t="n">
         <v>6</v>
@@ -969,7 +969,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>701.2</v>
+        <v>658.7</v>
       </c>
       <c r="C6" t="n">
         <v>4</v>
@@ -985,7 +985,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>419.8</v>
+        <v>457</v>
       </c>
       <c r="C7" t="n">
         <v>4</v>
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>254.7</v>
+        <v>375.5</v>
       </c>
       <c r="C8" t="n">
         <v>2</v>
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>201.6</v>
+        <v>207.2</v>
       </c>
       <c r="C9" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
feat: Enhance ETL pipeline to support SQL data extraction
- Updated `etl_main.py` to allow selection of data source (Excel or SQL) via command-line arguments.
- Modified `extract.py` to support data extraction from SQL databases using SQLAlchemy.
- Added connection handling for SQL databases, including error handling and table loading.
- Improved documentation and comments for clarity on new functionalities.
</commit_message>
<xml_diff>
--- a/reports/rapport_northwind.xlsx
+++ b/reports/rapport_northwind.xlsx
@@ -472,7 +472,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7416.700000000001</v>
+        <v>7655.499999999999</v>
       </c>
       <c r="B2" t="n">
         <v>48</v>
@@ -484,10 +484,10 @@
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>154.5145833333333</v>
+        <v>159.4895833333333</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8152173913043478</v>
+        <v>0.631578947368421</v>
       </c>
     </row>
   </sheetData>
@@ -544,13 +544,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>582.3</v>
+        <v>507.5</v>
       </c>
       <c r="D2" t="n">
         <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -561,13 +561,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>336.2</v>
+        <v>413.7</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
@@ -578,13 +578,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>1398.7</v>
+        <v>1331.2</v>
       </c>
       <c r="D4" t="n">
         <v>8</v>
       </c>
       <c r="E4" t="n">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5">
@@ -595,13 +595,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>2607.4</v>
+        <v>2796.1</v>
       </c>
       <c r="D5" t="n">
         <v>17</v>
       </c>
       <c r="E5" t="n">
-        <v>180</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6">
@@ -612,13 +612,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>1087.7</v>
+        <v>1027.6</v>
       </c>
       <c r="D6" t="n">
         <v>8</v>
       </c>
       <c r="E6" t="n">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
@@ -629,13 +629,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1404.4</v>
+        <v>1579.4</v>
       </c>
       <c r="D7" t="n">
         <v>8</v>
       </c>
       <c r="E7" t="n">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -686,13 +686,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4418.099999999999</v>
+        <v>4086</v>
       </c>
       <c r="C2" t="n">
         <v>48</v>
       </c>
       <c r="D2" t="n">
-        <v>265</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3">
@@ -702,13 +702,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2998.6</v>
+        <v>3569.5</v>
       </c>
       <c r="C3" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D3" t="n">
-        <v>243</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -759,10 +759,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4418.099999999999</v>
+        <v>4086</v>
       </c>
       <c r="C2" t="n">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="D2" t="n">
         <v>48</v>
@@ -775,13 +775,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1611.5</v>
+        <v>1787.5</v>
       </c>
       <c r="C3" t="n">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="D3" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -791,10 +791,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1387.1</v>
+        <v>1782</v>
       </c>
       <c r="C4" t="n">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="D4" t="n">
         <v>15</v>
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7416.7</v>
+        <v>7655.5</v>
       </c>
       <c r="C2" t="n">
         <v>48</v>
@@ -901,49 +901,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nancy Freehafer</t>
+          <t>Anne Hellung-Larsen</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2033.4</v>
+        <v>2263.2</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Anne Hellung-Larsen</t>
+          <t>Mariya Sergienko</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1410.1</v>
+        <v>1432.1</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mariya Sergienko</t>
+          <t>Nancy Freehafer</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1354.6</v>
+        <v>1365</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -953,7 +953,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>814.3</v>
+        <v>776.3000000000001</v>
       </c>
       <c r="C5" t="n">
         <v>6</v>
@@ -965,65 +965,65 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Robert Zare</t>
+          <t>Andrew Cencini</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>486</v>
+        <v>699</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Andrew Cencini</t>
+          <t>Laura Giussani</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>465.8</v>
+        <v>488.7</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Michael Neipper</t>
+          <t>Robert Zare</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>449.1</v>
+        <v>384.3</v>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Laura Giussani</t>
+          <t>Michael Neipper</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>403.4</v>
+        <v>246.9</v>
       </c>
       <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
         <v>2</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Enhance Northwind Dashboard with 3D delivery visualization and improve order simulation
- Added a new 3D plot for visualizing delivered vs non-delivered orders in the NorthwindDashboard.
- Updated the dashboard layout to include the new delivery visualization.
- Improved the order simulation process in the extractor by using a deterministic approach for product selection based on OrderID.
- Enhanced the transform script to maintain a 'WasShipped' indicator based on the presence of ShippedDate.
- Updated relevant documentation and comments for clarity.
</commit_message>
<xml_diff>
--- a/reports/rapport_northwind.xlsx
+++ b/reports/rapport_northwind.xlsx
@@ -472,7 +472,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7655.499999999999</v>
+        <v>8340.884000000002</v>
       </c>
       <c r="B2" t="n">
         <v>48</v>
@@ -481,13 +481,13 @@
         <v>15</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="E2" t="n">
-        <v>159.4895833333333</v>
+        <v>173.7684166666667</v>
       </c>
       <c r="F2" t="n">
-        <v>0.631578947368421</v>
+        <v>0.9895833333333334</v>
       </c>
     </row>
   </sheetData>
@@ -544,13 +544,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>507.5</v>
+        <v>707.735</v>
       </c>
       <c r="D2" t="n">
         <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
@@ -561,13 +561,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>413.7</v>
+        <v>508.5125000000001</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
@@ -578,13 +578,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>1331.2</v>
+        <v>1340.185</v>
       </c>
       <c r="D4" t="n">
         <v>8</v>
       </c>
       <c r="E4" t="n">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5">
@@ -595,13 +595,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>2796.1</v>
+        <v>3608.8235</v>
       </c>
       <c r="D5" t="n">
         <v>17</v>
       </c>
       <c r="E5" t="n">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6">
@@ -612,13 +612,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>1027.6</v>
+        <v>1239.578</v>
       </c>
       <c r="D6" t="n">
         <v>8</v>
       </c>
       <c r="E6" t="n">
-        <v>67</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7">
@@ -629,13 +629,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1579.4</v>
+        <v>936.05</v>
       </c>
       <c r="D7" t="n">
         <v>8</v>
       </c>
       <c r="E7" t="n">
-        <v>115</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -649,7 +649,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -682,33 +682,257 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Beverages</t>
+          <t>Jams, Preserves</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4086</v>
+        <v>1728.4</v>
       </c>
       <c r="C2" t="n">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>245</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Dried Fruit &amp; Nuts</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1490.4875</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11</v>
+      </c>
+      <c r="D3" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sauces</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1086.825</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Beverages</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>755.6279999999999</v>
+      </c>
+      <c r="C5" t="n">
+        <v>11</v>
+      </c>
+      <c r="D5" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Pasta</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>648.675</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Dairy Products</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>617.7</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>Condiments</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>3569.5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>32</v>
-      </c>
-      <c r="D3" t="n">
-        <v>282</v>
+      <c r="B8" t="n">
+        <v>466.9</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Baked Goods &amp; Mixes</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>444.821</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Candy</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>296.4375</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>235.2</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Canned Meat</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>206.28</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Oil</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>146.2475</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Canned Fruit &amp; Vegetables</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>81.59</v>
+      </c>
+      <c r="C14" t="n">
+        <v>11</v>
+      </c>
+      <c r="D14" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Cereal</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>68</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Chips, Snacks</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>45.45</v>
+      </c>
+      <c r="C16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Soups</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>22.2425</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -722,7 +946,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -755,49 +979,321 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Northwind Traders Chai</t>
+          <t>Northwind Traders Marmalade</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4086</v>
+        <v>1227.15</v>
       </c>
       <c r="C2" t="n">
-        <v>245</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
-        <v>48</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Northwind Traders Syrup</t>
+          <t>Northwind Traders Curry Sauce</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1787.5</v>
+        <v>780</v>
       </c>
       <c r="C3" t="n">
-        <v>192</v>
+        <v>20</v>
       </c>
       <c r="D3" t="n">
-        <v>32</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Northwind Traders Walnuts</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>645.1875</v>
+      </c>
+      <c r="C4" t="n">
+        <v>32</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Northwind Traders Mozzarella</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>617.7</v>
+      </c>
+      <c r="C5" t="n">
+        <v>19</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Northwind Traders Boysenberry Spread</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>501.25</v>
+      </c>
+      <c r="C6" t="n">
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Northwind Traders Dried Pears</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>403.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>14</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Northwind Traders Coffee</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>393.3</v>
+      </c>
+      <c r="C8" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Northwind Traders Ravioli</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>363.675</v>
+      </c>
+      <c r="C9" t="n">
+        <v>21</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Northwind Traders Dried Apples</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>302.1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>6</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Northwind Traders Chocolate</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>296.4375</v>
+      </c>
+      <c r="C11" t="n">
+        <v>24</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Northwind Traders Gnocchi</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>285</v>
+      </c>
+      <c r="C12" t="n">
+        <v>8</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>Northwind Traders Cajun Seasoning</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>1782</v>
-      </c>
-      <c r="C4" t="n">
-        <v>90</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="B13" t="n">
+        <v>284.9</v>
+      </c>
+      <c r="C13" t="n">
         <v>15</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Northwind Traders Long Grain Rice</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>235.2</v>
+      </c>
+      <c r="C14" t="n">
+        <v>36</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Northwind Traders Mustard</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>182</v>
+      </c>
+      <c r="C15" t="n">
+        <v>16</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Northwind Traders Scones</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>171</v>
+      </c>
+      <c r="C16" t="n">
+        <v>18</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Northwind Traders Tomato Sauce</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>170</v>
+      </c>
+      <c r="C17" t="n">
+        <v>10</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Northwind Traders Brownie Mix</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>161.121</v>
+      </c>
+      <c r="C18" t="n">
+        <v>14</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Northwind Traders Crab Meat</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>160.08</v>
+      </c>
+      <c r="C19" t="n">
+        <v>9</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Northwind Traders Olive Oil</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>146.2475</v>
+      </c>
+      <c r="C20" t="n">
+        <v>8</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Northwind Traders Hot Pepper Sauce</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>136.825</v>
+      </c>
+      <c r="C21" t="n">
+        <v>7</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +1344,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7655.5</v>
+        <v>8340.884</v>
       </c>
       <c r="C2" t="n">
         <v>48</v>
@@ -901,107 +1397,107 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Anne Hellung-Larsen</t>
+          <t>Nancy Freehafer</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2263.2</v>
+        <v>1792.0455</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mariya Sergienko</t>
+          <t>Anne Hellung-Larsen</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1432.1</v>
+        <v>1700.465</v>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nancy Freehafer</t>
+          <t>Jan Kotas</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1365</v>
+        <v>1504.468</v>
       </c>
       <c r="C4" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jan Kotas</t>
+          <t>Mariya Sergienko</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>776.3000000000001</v>
+        <v>1228.9555</v>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Andrew Cencini</t>
+          <t>Michael Neipper</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>699</v>
+        <v>931.827</v>
       </c>
       <c r="C6" t="n">
         <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Laura Giussani</t>
+          <t>Andrew Cencini</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>488.7</v>
+        <v>773.9504999999999</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Robert Zare</t>
+          <t>Laura Giussani</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>384.3</v>
+        <v>213.86</v>
       </c>
       <c r="C8" t="n">
         <v>2</v>
@@ -1013,17 +1509,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Michael Neipper</t>
+          <t>Robert Zare</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>246.9</v>
+        <v>195.3125</v>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>